<commit_message>
Core activaton summary module added.
</commit_message>
<xml_diff>
--- a/public/download/sample/Users.xlsx
+++ b/public/download/sample/Users.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="165">
   <si>
     <t>DD Code</t>
   </si>
@@ -46,7 +46,7 @@
     <t>faijul</t>
   </si>
   <si>
-    <t>01935593311</t>
+    <t>01900000001</t>
   </si>
   <si>
     <t>faijul@gmail.com</t>
@@ -61,7 +61,7 @@
     <t>forhad</t>
   </si>
   <si>
-    <t>01935591837</t>
+    <t>01900000002</t>
   </si>
   <si>
     <t>forhad@gmail.com</t>
@@ -73,7 +73,7 @@
     <t>joynal</t>
   </si>
   <si>
-    <t>01935591912</t>
+    <t>01900000003</t>
   </si>
   <si>
     <t>joynal@gmail.com</t>
@@ -85,7 +85,7 @@
     <t>md. golam mostufa</t>
   </si>
   <si>
-    <t>01935591856</t>
+    <t>01900000004</t>
   </si>
   <si>
     <t>md.golammostufa@gmail.com</t>
@@ -97,7 +97,7 @@
     <t>nazmul ahmed</t>
   </si>
   <si>
-    <t>01935592000</t>
+    <t>01900000005</t>
   </si>
   <si>
     <t>nazmulahmed@gmail.com</t>
@@ -109,7 +109,7 @@
     <t>porosh</t>
   </si>
   <si>
-    <t>01935591796</t>
+    <t>01900000006</t>
   </si>
   <si>
     <t>porosh@gmail.com</t>
@@ -121,7 +121,7 @@
     <t>md. anik hasan</t>
   </si>
   <si>
-    <t>01935591917</t>
+    <t>01900000007</t>
   </si>
   <si>
     <t>md.anikhasan@gmail.com</t>
@@ -133,7 +133,7 @@
     <t>md. siyam hossain</t>
   </si>
   <si>
-    <t>01935591855</t>
+    <t>01900000008</t>
   </si>
   <si>
     <t>md.siyamhossain@gmail.com</t>
@@ -145,7 +145,7 @@
     <t>habibur rahman</t>
   </si>
   <si>
-    <t>01935592053</t>
+    <t>01900000009</t>
   </si>
   <si>
     <t>habiburrahman@gmail.com</t>
@@ -157,7 +157,7 @@
     <t>mizan</t>
   </si>
   <si>
-    <t>01935591915</t>
+    <t>01900000010</t>
   </si>
   <si>
     <t>mizan@gmail.com</t>
@@ -172,7 +172,7 @@
     <t>rakib mia</t>
   </si>
   <si>
-    <t>01935593313</t>
+    <t>01900000011</t>
   </si>
   <si>
     <t>rakibmia@gmail.com</t>
@@ -184,7 +184,7 @@
     <t>abdullah al alam</t>
   </si>
   <si>
-    <t>01935591816</t>
+    <t>01900000012</t>
   </si>
   <si>
     <t>abdullahalalam@gmail.com</t>
@@ -196,7 +196,7 @@
     <t>shakil</t>
   </si>
   <si>
-    <t>01935591916</t>
+    <t>01900000013</t>
   </si>
   <si>
     <t>shakil@gmail.com</t>
@@ -208,7 +208,7 @@
     <t>md. jubayed mia</t>
   </si>
   <si>
-    <t>01935592484</t>
+    <t>01900000014</t>
   </si>
   <si>
     <t>md.jubayedmia@gmail.com</t>
@@ -220,7 +220,7 @@
     <t>md. monir hossen</t>
   </si>
   <si>
-    <t>01935591836</t>
+    <t>01900000015</t>
   </si>
   <si>
     <t>md.monirhossen@gmail.com</t>
@@ -232,7 +232,7 @@
     <t>md. shahin mia</t>
   </si>
   <si>
-    <t>01935591828</t>
+    <t>01900000016</t>
   </si>
   <si>
     <t>md.shahinmia@gmail.com</t>
@@ -244,7 +244,7 @@
     <t>ashiqur rahman</t>
   </si>
   <si>
-    <t>01935592119</t>
+    <t>01900000017</t>
   </si>
   <si>
     <t>ashiqurrahman@gmail.com</t>
@@ -259,7 +259,7 @@
     <t>safiqul islam</t>
   </si>
   <si>
-    <t>01935593312</t>
+    <t>01900000018</t>
   </si>
   <si>
     <t>safiqulislam@gmail.com</t>
@@ -271,7 +271,7 @@
     <t>saddam</t>
   </si>
   <si>
-    <t>01935591829</t>
+    <t>01900000019</t>
   </si>
   <si>
     <t>saddam@gmail.com</t>
@@ -283,7 +283,7 @@
     <t>md. bayazid</t>
   </si>
   <si>
-    <t>01935591914</t>
+    <t>01900000020</t>
   </si>
   <si>
     <t>md.bayazid@gmail.com</t>
@@ -295,7 +295,7 @@
     <t>saikoutz zaman raja</t>
   </si>
   <si>
-    <t>01935591815</t>
+    <t>01900000021</t>
   </si>
   <si>
     <t>saikoutzzamanraja@gmail.com</t>
@@ -307,7 +307,7 @@
     <t>md. thouhul amin</t>
   </si>
   <si>
-    <t>01935591797</t>
+    <t>01900000022</t>
   </si>
   <si>
     <t>md.thouhulamin@gmail.com</t>
@@ -319,7 +319,7 @@
     <t>monayam khan</t>
   </si>
   <si>
-    <t>01935591918</t>
+    <t>01900000023</t>
   </si>
   <si>
     <t>monayamkhan@gmail.com</t>
@@ -331,7 +331,7 @@
     <t>mohammd abul hossain</t>
   </si>
   <si>
-    <t>01935591999</t>
+    <t>01900000024</t>
   </si>
   <si>
     <t>mohammdabulhossain@gmail.com</t>
@@ -343,7 +343,7 @@
     <t>hridoy mia</t>
   </si>
   <si>
-    <t>01935591913</t>
+    <t>01900000025</t>
   </si>
   <si>
     <t>hridoymia@gmail.com</t>
@@ -355,10 +355,160 @@
     <t>md. hridoy mia</t>
   </si>
   <si>
-    <t>01935592054</t>
+    <t>01900000026</t>
   </si>
   <si>
     <t>md.hridoymia@gmail.com</t>
+  </si>
+  <si>
+    <t>Titu Miah</t>
+  </si>
+  <si>
+    <t>titumiah</t>
+  </si>
+  <si>
+    <t>01900000027</t>
+  </si>
+  <si>
+    <t>titumiah@gmail.com</t>
+  </si>
+  <si>
+    <t>supervisor</t>
+  </si>
+  <si>
+    <t>Ridoy Miah</t>
+  </si>
+  <si>
+    <t>ridoymiah</t>
+  </si>
+  <si>
+    <t>01900000028</t>
+  </si>
+  <si>
+    <t>ridoymiah@gmail.com</t>
+  </si>
+  <si>
+    <t>Ruhul Amin</t>
+  </si>
+  <si>
+    <t>ruhulamin</t>
+  </si>
+  <si>
+    <t>01900000029</t>
+  </si>
+  <si>
+    <t>ruhulamin@gmail.com</t>
+  </si>
+  <si>
+    <t>Supervisor One</t>
+  </si>
+  <si>
+    <t>supervisor01</t>
+  </si>
+  <si>
+    <t>01900000030</t>
+  </si>
+  <si>
+    <t>supervisor01@gmail.com</t>
+  </si>
+  <si>
+    <t>Supervisor Two</t>
+  </si>
+  <si>
+    <t>supervisor02</t>
+  </si>
+  <si>
+    <t>01900000031</t>
+  </si>
+  <si>
+    <t>supervisor02@gmail.com</t>
+  </si>
+  <si>
+    <t>Supervisor Three</t>
+  </si>
+  <si>
+    <t>supervisor03</t>
+  </si>
+  <si>
+    <t>01900000032</t>
+  </si>
+  <si>
+    <t>supervisor03@gmail.com</t>
+  </si>
+  <si>
+    <t>BP 01</t>
+  </si>
+  <si>
+    <t>bp01</t>
+  </si>
+  <si>
+    <t>01900000033</t>
+  </si>
+  <si>
+    <t>bp01@gmail.com</t>
+  </si>
+  <si>
+    <t>bp</t>
+  </si>
+  <si>
+    <t>BP 02</t>
+  </si>
+  <si>
+    <t>bp02</t>
+  </si>
+  <si>
+    <t>01900000034</t>
+  </si>
+  <si>
+    <t>bp02@gmail.com</t>
+  </si>
+  <si>
+    <t>BP 03</t>
+  </si>
+  <si>
+    <t>bp03</t>
+  </si>
+  <si>
+    <t>01900000035</t>
+  </si>
+  <si>
+    <t>bp03@gmail.com</t>
+  </si>
+  <si>
+    <t>BP 04</t>
+  </si>
+  <si>
+    <t>bp04</t>
+  </si>
+  <si>
+    <t>01900000036</t>
+  </si>
+  <si>
+    <t>bp04@gmail.com</t>
+  </si>
+  <si>
+    <t>BP 05</t>
+  </si>
+  <si>
+    <t>bp05</t>
+  </si>
+  <si>
+    <t>01900000037</t>
+  </si>
+  <si>
+    <t>bp05@gmail.com</t>
+  </si>
+  <si>
+    <t>BP 06</t>
+  </si>
+  <si>
+    <t>bp06</t>
+  </si>
+  <si>
+    <t>01900000038</t>
+  </si>
+  <si>
+    <t>bp06@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -366,10 +516,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -396,6 +546,43 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -412,52 +599,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -466,36 +617,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -510,6 +631,22 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -517,9 +654,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -531,6 +674,13 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -541,25 +691,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -571,157 +847,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -738,23 +888,41 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -774,11 +942,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -808,44 +982,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -858,127 +1008,127 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -993,6 +1143,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1314,10 +1467,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F31" sqref="A1:G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="6"/>
@@ -1327,7 +1480,7 @@
     <col min="3" max="3" width="24.1428571428571" style="2" customWidth="1"/>
     <col min="4" max="4" width="12.8571428571429" style="2" customWidth="1"/>
     <col min="5" max="5" width="35.5714285714286" style="2" customWidth="1"/>
-    <col min="6" max="6" width="5.57142857142857" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11" style="2" customWidth="1"/>
     <col min="7" max="7" width="10" style="2" customWidth="1"/>
     <col min="8" max="16384" width="9.14285714285714" style="2"/>
   </cols>
@@ -1365,7 +1518,7 @@
       <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -1388,7 +1541,7 @@
       <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -1411,7 +1564,7 @@
       <c r="C4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -1434,7 +1587,7 @@
       <c r="C5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -1457,7 +1610,7 @@
       <c r="C6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -1480,7 +1633,7 @@
       <c r="C7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -1503,7 +1656,7 @@
       <c r="C8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="4" t="s">
         <v>35</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -1526,7 +1679,7 @@
       <c r="C9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -1549,7 +1702,7 @@
       <c r="C10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="4" t="s">
         <v>43</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -1572,7 +1725,7 @@
       <c r="C11" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="4" t="s">
         <v>47</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -1595,7 +1748,7 @@
       <c r="C12" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="4" t="s">
         <v>52</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -1618,7 +1771,7 @@
       <c r="C13" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="4" t="s">
         <v>56</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -1641,7 +1794,7 @@
       <c r="C14" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E14" s="2" t="s">
@@ -1664,7 +1817,7 @@
       <c r="C15" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="4" t="s">
         <v>64</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -1687,7 +1840,7 @@
       <c r="C16" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E16" s="3" t="s">
@@ -1710,7 +1863,7 @@
       <c r="C17" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="4" t="s">
         <v>72</v>
       </c>
       <c r="E17" s="3" t="s">
@@ -1733,7 +1886,7 @@
       <c r="C18" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="4" t="s">
         <v>76</v>
       </c>
       <c r="E18" s="3" t="s">
@@ -1756,7 +1909,7 @@
       <c r="C19" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="4" t="s">
         <v>81</v>
       </c>
       <c r="E19" s="3" t="s">
@@ -1779,7 +1932,7 @@
       <c r="C20" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="4" t="s">
         <v>85</v>
       </c>
       <c r="E20" s="2" t="s">
@@ -1802,7 +1955,7 @@
       <c r="C21" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="4" t="s">
         <v>89</v>
       </c>
       <c r="E21" s="3" t="s">
@@ -1825,7 +1978,7 @@
       <c r="C22" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="4" t="s">
         <v>93</v>
       </c>
       <c r="E22" s="3" t="s">
@@ -1848,7 +2001,7 @@
       <c r="C23" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="4" t="s">
         <v>97</v>
       </c>
       <c r="E23" s="3" t="s">
@@ -1871,7 +2024,7 @@
       <c r="C24" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="4" t="s">
         <v>101</v>
       </c>
       <c r="E24" s="3" t="s">
@@ -1894,7 +2047,7 @@
       <c r="C25" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="4" t="s">
         <v>105</v>
       </c>
       <c r="E25" s="3" t="s">
@@ -1917,7 +2070,7 @@
       <c r="C26" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="4" t="s">
         <v>109</v>
       </c>
       <c r="E26" s="3" t="s">
@@ -1940,7 +2093,7 @@
       <c r="C27" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="4" t="s">
         <v>113</v>
       </c>
       <c r="E27" s="3" t="s">
@@ -1950,6 +2103,282 @@
         <v>12</v>
       </c>
       <c r="G27" s="2">
+        <v>32133213</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G28" s="2">
+        <v>32133213</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G29" s="2">
+        <v>32133213</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G30" s="2">
+        <v>32133213</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G31" s="2">
+        <v>32133213</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G32" s="2">
+        <v>32133213</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G33" s="2">
+        <v>32133213</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G34" s="2">
+        <v>32133213</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G35" s="2">
+        <v>32133213</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G36" s="2">
+        <v>32133213</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G37" s="2">
+        <v>32133213</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G38" s="2">
+        <v>32133213</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G39" s="2">
         <v>32133213</v>
       </c>
     </row>
@@ -1974,6 +2403,18 @@
     <hyperlink ref="E25" r:id="rId17" display="mohammdabulhossain@gmail.com"/>
     <hyperlink ref="E26" r:id="rId18" display="hridoymia@gmail.com"/>
     <hyperlink ref="E27" r:id="rId19" display="md.hridoymia@gmail.com"/>
+    <hyperlink ref="E28" r:id="rId20" display="titumiah@gmail.com"/>
+    <hyperlink ref="E29" r:id="rId21" display="ridoymiah@gmail.com"/>
+    <hyperlink ref="E30" r:id="rId22" display="ruhulamin@gmail.com"/>
+    <hyperlink ref="E34" r:id="rId23" display="bp01@gmail.com"/>
+    <hyperlink ref="E35" r:id="rId23" display="bp02@gmail.com"/>
+    <hyperlink ref="E36" r:id="rId23" display="bp03@gmail.com"/>
+    <hyperlink ref="E37" r:id="rId23" display="bp04@gmail.com"/>
+    <hyperlink ref="E38" r:id="rId23" display="bp05@gmail.com"/>
+    <hyperlink ref="E39" r:id="rId23" display="bp06@gmail.com"/>
+    <hyperlink ref="E31" r:id="rId24" display="supervisor01@gmail.com"/>
+    <hyperlink ref="E32" r:id="rId24" display="supervisor02@gmail.com"/>
+    <hyperlink ref="E33" r:id="rId24" display="supervisor03@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>